<commit_message>
Add more Java code
</commit_message>
<xml_diff>
--- a/variable list.xlsx
+++ b/variable list.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="75">
   <si>
     <t>Score</t>
   </si>
@@ -51,13 +52,211 @@
   </si>
   <si>
     <t>frameTotalScoresPlayer2[10]</t>
+  </si>
+  <si>
+    <t>frame1Score2Player1</t>
+  </si>
+  <si>
+    <t>frame2Score1Player1</t>
+  </si>
+  <si>
+    <t>frame2Score2Player1</t>
+  </si>
+  <si>
+    <t>frame3Score1Player1</t>
+  </si>
+  <si>
+    <t>frame3Score2Player1</t>
+  </si>
+  <si>
+    <t>frame4Score1Player1</t>
+  </si>
+  <si>
+    <t>frame4Score2Player1</t>
+  </si>
+  <si>
+    <t>frame5Score1Player1</t>
+  </si>
+  <si>
+    <t>frame5Score2Player1</t>
+  </si>
+  <si>
+    <t>frame6Score1Player1</t>
+  </si>
+  <si>
+    <t>frame6Score2Player1</t>
+  </si>
+  <si>
+    <t>frame7Score1Player1</t>
+  </si>
+  <si>
+    <t>frame7Score2Player1</t>
+  </si>
+  <si>
+    <t>frame8Score1Player1</t>
+  </si>
+  <si>
+    <t>frame8Score2Player1</t>
+  </si>
+  <si>
+    <t>frame9Score1Player1</t>
+  </si>
+  <si>
+    <t>frame9Score2Player1</t>
+  </si>
+  <si>
+    <t>frame10Score1Player1</t>
+  </si>
+  <si>
+    <t>frame10Score2Player1</t>
+  </si>
+  <si>
+    <t>frame10Score3Player1</t>
+  </si>
+  <si>
+    <t>frame1Score1Player2</t>
+  </si>
+  <si>
+    <t>frame1Score2Player2</t>
+  </si>
+  <si>
+    <t>frame2Score1Player2</t>
+  </si>
+  <si>
+    <t>frame2Score2Player2</t>
+  </si>
+  <si>
+    <t>frame3Score1Player2</t>
+  </si>
+  <si>
+    <t>frame3Score2Player2</t>
+  </si>
+  <si>
+    <t>frame4Score1Player2</t>
+  </si>
+  <si>
+    <t>frame4Score2Player2</t>
+  </si>
+  <si>
+    <t>frame5Score1Player2</t>
+  </si>
+  <si>
+    <t>frame5Score2Player2</t>
+  </si>
+  <si>
+    <t>frame6Score1Player2</t>
+  </si>
+  <si>
+    <t>frame6Score2Player2</t>
+  </si>
+  <si>
+    <t>frame7Score1Player2</t>
+  </si>
+  <si>
+    <t>frame7Score2Player2</t>
+  </si>
+  <si>
+    <t>frame8Score1Player2</t>
+  </si>
+  <si>
+    <t>frame8Score2Player2</t>
+  </si>
+  <si>
+    <t>frame9Score1Player2</t>
+  </si>
+  <si>
+    <t>frame9Score2Player2</t>
+  </si>
+  <si>
+    <t>frame10Score1Player2</t>
+  </si>
+  <si>
+    <t>frame10Score2Player2</t>
+  </si>
+  <si>
+    <t>frame10Score3Player2</t>
+  </si>
+  <si>
+    <t>frame1TotalScorePlayer1</t>
+  </si>
+  <si>
+    <t>frame2TotalScorePlayer1</t>
+  </si>
+  <si>
+    <t>frame3TotalScorePlayer1</t>
+  </si>
+  <si>
+    <t>frame4TotalScorePlayer1</t>
+  </si>
+  <si>
+    <t>frame5TotalScorePlayer1</t>
+  </si>
+  <si>
+    <t>frame6TotalScorePlayer1</t>
+  </si>
+  <si>
+    <t>frame7TotalScorePlayer1</t>
+  </si>
+  <si>
+    <t>frame8TotalScorePlayer1</t>
+  </si>
+  <si>
+    <t>frame9TotalScorePlayer1</t>
+  </si>
+  <si>
+    <t>frame10TotalScorePlayer1</t>
+  </si>
+  <si>
+    <t>frame1TotalScorePlayer2</t>
+  </si>
+  <si>
+    <t>frame2TotalScorePlayer2</t>
+  </si>
+  <si>
+    <t>frame3TotalScorePlayer2</t>
+  </si>
+  <si>
+    <t>frame4TotalScorePlayer2</t>
+  </si>
+  <si>
+    <t>frame5TotalScorePlayer2</t>
+  </si>
+  <si>
+    <t>frame6TotalScorePlayer2</t>
+  </si>
+  <si>
+    <t>frame7TotalScorePlayer2</t>
+  </si>
+  <si>
+    <t>frame8TotalScorePlayer2</t>
+  </si>
+  <si>
+    <t>frame9TotalScorePlayer2</t>
+  </si>
+  <si>
+    <t>frame10TotalScorePlayer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TextView </t>
+  </si>
+  <si>
+    <t>frameScoresPlayer1[</t>
+  </si>
+  <si>
+    <t>frameScoresPlayer2[</t>
+  </si>
+  <si>
+    <t>frameTotalScoresPlayer1[</t>
+  </si>
+  <si>
+    <t>frameTotalScoresPlayer2[</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +270,11 @@
       <color rgb="FF6A8759"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF303336"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,10 +297,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -412,28 +619,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N70" sqref="N3:N70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="57.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="I2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -459,8 +668,19 @@
       <c r="I3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" t="str">
+        <f>J3&amp;I3&amp;"]"</f>
+        <v>frameScoresPlayer1[1]</v>
+      </c>
+      <c r="N3" s="2" t="str">
+        <f>H3&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;L3&amp;");"</f>
+        <v>frame1Score1Player1.setText(""+frameScoresPlayer1[1]);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -486,8 +706,19 @@
       <c r="I4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" ref="L4:L23" si="1">J4&amp;I4&amp;"]"</f>
+        <v>frameScoresPlayer1[2]</v>
+      </c>
+      <c r="N4" s="2" t="str">
+        <f t="shared" ref="N4:N23" si="2">H4&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;L4&amp;");"</f>
+        <v>frame1Score2Player1.setText(""+frameScoresPlayer1[2]);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -513,8 +744,19 @@
       <c r="I5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[3]</v>
+      </c>
+      <c r="N5" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame2Score1Player1.setText(""+frameScoresPlayer1[3]);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -540,8 +782,19 @@
       <c r="I6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>71</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[4]</v>
+      </c>
+      <c r="N6" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame2Score2Player1.setText(""+frameScoresPlayer1[4]);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -567,8 +820,19 @@
       <c r="I7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>71</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[5]</v>
+      </c>
+      <c r="N7" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame3Score1Player1.setText(""+frameScoresPlayer1[5]);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -594,8 +858,19 @@
       <c r="I8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>71</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[6]</v>
+      </c>
+      <c r="N8" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame3Score2Player1.setText(""+frameScoresPlayer1[6]);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -621,8 +896,19 @@
       <c r="I9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>71</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[7]</v>
+      </c>
+      <c r="N9" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame4Score1Player1.setText(""+frameScoresPlayer1[7]);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -648,8 +934,19 @@
       <c r="I10">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[8]</v>
+      </c>
+      <c r="N10" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame4Score2Player1.setText(""+frameScoresPlayer1[8]);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -675,8 +972,19 @@
       <c r="I11">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[9]</v>
+      </c>
+      <c r="N11" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame5Score1Player1.setText(""+frameScoresPlayer1[9]);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -702,8 +1010,19 @@
       <c r="I12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>71</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[10]</v>
+      </c>
+      <c r="N12" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame5Score2Player1.setText(""+frameScoresPlayer1[10]);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -729,8 +1048,19 @@
       <c r="I13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>71</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[11]</v>
+      </c>
+      <c r="N13" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame6Score1Player1.setText(""+frameScoresPlayer1[11]);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -756,8 +1086,19 @@
       <c r="I14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>71</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[12]</v>
+      </c>
+      <c r="N14" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame6Score2Player1.setText(""+frameScoresPlayer1[12]);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -783,8 +1124,19 @@
       <c r="I15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>71</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[13]</v>
+      </c>
+      <c r="N15" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame7Score1Player1.setText(""+frameScoresPlayer1[13]);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -810,8 +1162,19 @@
       <c r="I16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>71</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[14]</v>
+      </c>
+      <c r="N16" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame7Score2Player1.setText(""+frameScoresPlayer1[14]);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -837,8 +1200,19 @@
       <c r="I17">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>71</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[15]</v>
+      </c>
+      <c r="N17" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame8Score1Player1.setText(""+frameScoresPlayer1[15]);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -864,8 +1238,19 @@
       <c r="I18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>71</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[16]</v>
+      </c>
+      <c r="N18" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame8Score2Player1.setText(""+frameScoresPlayer1[16]);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -891,8 +1276,19 @@
       <c r="I19">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>71</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[17]</v>
+      </c>
+      <c r="N19" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame9Score1Player1.setText(""+frameScoresPlayer1[17]);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -918,8 +1314,19 @@
       <c r="I20">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>71</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[18]</v>
+      </c>
+      <c r="N20" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame9Score2Player1.setText(""+frameScoresPlayer1[18]);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -945,8 +1352,19 @@
       <c r="I21">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>71</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[19]</v>
+      </c>
+      <c r="N21" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame10Score1Player1.setText(""+frameScoresPlayer1[19]);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -972,8 +1390,19 @@
       <c r="I22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>71</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[20]</v>
+      </c>
+      <c r="N22" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame10Score2Player1.setText(""+frameScoresPlayer1[20]);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -999,13 +1428,24 @@
       <c r="I23">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>71</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="1"/>
+        <v>frameScoresPlayer1[21]</v>
+      </c>
+      <c r="N23" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>frame10Score3Player1.setText(""+frameScoresPlayer1[21]);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="I25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -1031,8 +1471,19 @@
       <c r="I26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>72</v>
+      </c>
+      <c r="L26" t="str">
+        <f>J26&amp;I26&amp;"]"</f>
+        <v>frameScoresPlayer2[1]</v>
+      </c>
+      <c r="N26" s="2" t="str">
+        <f>H26&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;L26&amp;");"</f>
+        <v>frame1Score1Player2.setText(""+frameScoresPlayer2[1]);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1058,8 +1509,19 @@
       <c r="I27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>72</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" ref="L27:L46" si="3">J27&amp;I27&amp;"]"</f>
+        <v>frameScoresPlayer2[2]</v>
+      </c>
+      <c r="N27" s="2" t="str">
+        <f t="shared" ref="N27:N46" si="4">H27&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;L27&amp;");"</f>
+        <v>frame1Score2Player2.setText(""+frameScoresPlayer2[2]);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1085,8 +1547,19 @@
       <c r="I28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[3]</v>
+      </c>
+      <c r="N28" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame2Score1Player2.setText(""+frameScoresPlayer2[3]);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1112,8 +1585,19 @@
       <c r="I29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>72</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[4]</v>
+      </c>
+      <c r="N29" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame2Score2Player2.setText(""+frameScoresPlayer2[4]);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1139,8 +1623,19 @@
       <c r="I30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>72</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[5]</v>
+      </c>
+      <c r="N30" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame3Score1Player2.setText(""+frameScoresPlayer2[5]);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1166,8 +1661,19 @@
       <c r="I31">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>72</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[6]</v>
+      </c>
+      <c r="N31" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame3Score2Player2.setText(""+frameScoresPlayer2[6]);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1193,8 +1699,19 @@
       <c r="I32">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>72</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[7]</v>
+      </c>
+      <c r="N32" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame4Score1Player2.setText(""+frameScoresPlayer2[7]);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1220,8 +1737,19 @@
       <c r="I33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>72</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[8]</v>
+      </c>
+      <c r="N33" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame4Score2Player2.setText(""+frameScoresPlayer2[8]);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1247,8 +1775,19 @@
       <c r="I34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>72</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[9]</v>
+      </c>
+      <c r="N34" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame5Score1Player2.setText(""+frameScoresPlayer2[9]);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1274,8 +1813,19 @@
       <c r="I35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>72</v>
+      </c>
+      <c r="L35" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[10]</v>
+      </c>
+      <c r="N35" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame5Score2Player2.setText(""+frameScoresPlayer2[10]);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1301,8 +1851,19 @@
       <c r="I36">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>72</v>
+      </c>
+      <c r="L36" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[11]</v>
+      </c>
+      <c r="N36" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame6Score1Player2.setText(""+frameScoresPlayer2[11]);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1328,8 +1889,19 @@
       <c r="I37">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>72</v>
+      </c>
+      <c r="L37" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[12]</v>
+      </c>
+      <c r="N37" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame6Score2Player2.setText(""+frameScoresPlayer2[12]);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1355,8 +1927,19 @@
       <c r="I38">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>72</v>
+      </c>
+      <c r="L38" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[13]</v>
+      </c>
+      <c r="N38" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame7Score1Player2.setText(""+frameScoresPlayer2[13]);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1382,8 +1965,19 @@
       <c r="I39">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>72</v>
+      </c>
+      <c r="L39" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[14]</v>
+      </c>
+      <c r="N39" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame7Score2Player2.setText(""+frameScoresPlayer2[14]);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1409,8 +2003,19 @@
       <c r="I40">
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>72</v>
+      </c>
+      <c r="L40" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[15]</v>
+      </c>
+      <c r="N40" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame8Score1Player2.setText(""+frameScoresPlayer2[15]);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -1436,8 +2041,19 @@
       <c r="I41">
         <v>16</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>72</v>
+      </c>
+      <c r="L41" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[16]</v>
+      </c>
+      <c r="N41" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame8Score2Player2.setText(""+frameScoresPlayer2[16]);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -1463,8 +2079,19 @@
       <c r="I42">
         <v>17</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>72</v>
+      </c>
+      <c r="L42" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[17]</v>
+      </c>
+      <c r="N42" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame9Score1Player2.setText(""+frameScoresPlayer2[17]);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>4</v>
       </c>
@@ -1490,8 +2117,19 @@
       <c r="I43">
         <v>18</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>72</v>
+      </c>
+      <c r="L43" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[18]</v>
+      </c>
+      <c r="N43" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame9Score2Player2.setText(""+frameScoresPlayer2[18]);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
         <v>4</v>
       </c>
@@ -1517,8 +2155,19 @@
       <c r="I44">
         <v>19</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>72</v>
+      </c>
+      <c r="L44" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[19]</v>
+      </c>
+      <c r="N44" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame10Score1Player2.setText(""+frameScoresPlayer2[19]);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1544,8 +2193,19 @@
       <c r="I45">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>72</v>
+      </c>
+      <c r="L45" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[20]</v>
+      </c>
+      <c r="N45" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame10Score2Player2.setText(""+frameScoresPlayer2[20]);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -1571,13 +2231,24 @@
       <c r="I46">
         <v>21</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>72</v>
+      </c>
+      <c r="L46" t="str">
+        <f t="shared" si="3"/>
+        <v>frameScoresPlayer2[21]</v>
+      </c>
+      <c r="N46" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>frame10Score3Player2.setText(""+frameScoresPlayer2[21]);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="I48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -1594,14 +2265,25 @@
         <v>1</v>
       </c>
       <c r="H49" t="str">
-        <f t="shared" ref="H49:H58" si="1">A49&amp;B49&amp;C49&amp;D49&amp;E49&amp;F49</f>
+        <f t="shared" ref="H49:H58" si="5">A49&amp;B49&amp;C49&amp;D49&amp;E49&amp;F49</f>
         <v>frame1TotalScorePlayer1</v>
       </c>
       <c r="I49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>73</v>
+      </c>
+      <c r="L49" t="str">
+        <f t="shared" ref="L49:L70" si="6">J49&amp;I49&amp;"]"</f>
+        <v>frameTotalScoresPlayer1[1]</v>
+      </c>
+      <c r="N49" s="2" t="str">
+        <f t="shared" ref="N49:N58" si="7">H49&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;L49&amp;");"</f>
+        <v>frame1TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[1]);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -1618,14 +2300,25 @@
         <v>1</v>
       </c>
       <c r="H50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>frame2TotalScorePlayer1</v>
       </c>
       <c r="I50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>73</v>
+      </c>
+      <c r="L50" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer1[2]</v>
+      </c>
+      <c r="N50" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>frame2TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[2]);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -1642,14 +2335,25 @@
         <v>1</v>
       </c>
       <c r="H51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>frame3TotalScorePlayer1</v>
       </c>
       <c r="I51">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>73</v>
+      </c>
+      <c r="L51" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer1[3]</v>
+      </c>
+      <c r="N51" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>frame3TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[3]);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
       <c r="A52" t="s">
         <v>4</v>
       </c>
@@ -1666,14 +2370,25 @@
         <v>1</v>
       </c>
       <c r="H52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>frame4TotalScorePlayer1</v>
       </c>
       <c r="I52">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>73</v>
+      </c>
+      <c r="L52" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer1[4]</v>
+      </c>
+      <c r="N52" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>frame4TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[4]);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="A53" t="s">
         <v>4</v>
       </c>
@@ -1690,14 +2405,25 @@
         <v>1</v>
       </c>
       <c r="H53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>frame5TotalScorePlayer1</v>
       </c>
       <c r="I53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>73</v>
+      </c>
+      <c r="L53" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer1[5]</v>
+      </c>
+      <c r="N53" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>frame5TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[5]);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="A54" t="s">
         <v>4</v>
       </c>
@@ -1714,14 +2440,25 @@
         <v>1</v>
       </c>
       <c r="H54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>frame6TotalScorePlayer1</v>
       </c>
       <c r="I54">
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>73</v>
+      </c>
+      <c r="L54" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer1[6]</v>
+      </c>
+      <c r="N54" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>frame6TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[6]);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -1738,14 +2475,25 @@
         <v>1</v>
       </c>
       <c r="H55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>frame7TotalScorePlayer1</v>
       </c>
       <c r="I55">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>73</v>
+      </c>
+      <c r="L55" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer1[7]</v>
+      </c>
+      <c r="N55" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>frame7TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[7]);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -1762,14 +2510,25 @@
         <v>1</v>
       </c>
       <c r="H56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>frame8TotalScorePlayer1</v>
       </c>
       <c r="I56">
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>73</v>
+      </c>
+      <c r="L56" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer1[8]</v>
+      </c>
+      <c r="N56" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>frame8TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[8]);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
       <c r="A57" t="s">
         <v>4</v>
       </c>
@@ -1786,14 +2545,25 @@
         <v>1</v>
       </c>
       <c r="H57" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>frame9TotalScorePlayer1</v>
       </c>
       <c r="I57">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>73</v>
+      </c>
+      <c r="L57" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer1[9]</v>
+      </c>
+      <c r="N57" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>frame9TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[9]);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
       <c r="A58" t="s">
         <v>4</v>
       </c>
@@ -1810,19 +2580,30 @@
         <v>1</v>
       </c>
       <c r="H58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>frame10TotalScorePlayer1</v>
       </c>
       <c r="I58">
         <v>10</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>73</v>
+      </c>
+      <c r="L58" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer1[10]</v>
+      </c>
+      <c r="N58" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>frame10TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[10]);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
       <c r="I60" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -1839,14 +2620,25 @@
         <v>2</v>
       </c>
       <c r="H61" t="str">
-        <f t="shared" ref="H61:H70" si="2">A61&amp;B61&amp;C61&amp;D61&amp;E61&amp;F61</f>
+        <f t="shared" ref="H61:H70" si="8">A61&amp;B61&amp;C61&amp;D61&amp;E61&amp;F61</f>
         <v>frame1TotalScorePlayer2</v>
       </c>
       <c r="I61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>74</v>
+      </c>
+      <c r="L61" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer2[1]</v>
+      </c>
+      <c r="N61" s="2" t="str">
+        <f t="shared" ref="N61:N70" si="9">H61&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;L61&amp;");"</f>
+        <v>frame1TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[1]);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -1863,14 +2655,25 @@
         <v>2</v>
       </c>
       <c r="H62" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>frame2TotalScorePlayer2</v>
       </c>
       <c r="I62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>74</v>
+      </c>
+      <c r="L62" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer2[2]</v>
+      </c>
+      <c r="N62" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>frame2TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[2]);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -1887,14 +2690,25 @@
         <v>2</v>
       </c>
       <c r="H63" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>frame3TotalScorePlayer2</v>
       </c>
       <c r="I63">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>74</v>
+      </c>
+      <c r="L63" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer2[3]</v>
+      </c>
+      <c r="N63" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>frame3TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[3]);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -1911,14 +2725,25 @@
         <v>2</v>
       </c>
       <c r="H64" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>frame4TotalScorePlayer2</v>
       </c>
       <c r="I64">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>74</v>
+      </c>
+      <c r="L64" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer2[4]</v>
+      </c>
+      <c r="N64" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>frame4TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[4]);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -1935,14 +2760,25 @@
         <v>2</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>frame5TotalScorePlayer2</v>
       </c>
       <c r="I65">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>74</v>
+      </c>
+      <c r="L65" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer2[5]</v>
+      </c>
+      <c r="N65" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>frame5TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[5]);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -1959,14 +2795,25 @@
         <v>2</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>frame6TotalScorePlayer2</v>
       </c>
       <c r="I66">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>74</v>
+      </c>
+      <c r="L66" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer2[6]</v>
+      </c>
+      <c r="N66" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>frame6TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[6]);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -1983,14 +2830,25 @@
         <v>2</v>
       </c>
       <c r="H67" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>frame7TotalScorePlayer2</v>
       </c>
       <c r="I67">
         <v>7</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>74</v>
+      </c>
+      <c r="L67" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer2[7]</v>
+      </c>
+      <c r="N67" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>frame7TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[7]);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -2007,14 +2865,25 @@
         <v>2</v>
       </c>
       <c r="H68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>frame8TotalScorePlayer2</v>
       </c>
       <c r="I68">
         <v>8</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>74</v>
+      </c>
+      <c r="L68" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer2[8]</v>
+      </c>
+      <c r="N68" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>frame8TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[8]);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
       <c r="A69" t="s">
         <v>4</v>
       </c>
@@ -2031,14 +2900,25 @@
         <v>2</v>
       </c>
       <c r="H69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>frame9TotalScorePlayer2</v>
       </c>
       <c r="I69">
         <v>9</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>74</v>
+      </c>
+      <c r="L69" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer2[9]</v>
+      </c>
+      <c r="N69" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>frame9TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[9]);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -2055,11 +2935,1034 @@
         <v>2</v>
       </c>
       <c r="H70" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>frame10TotalScorePlayer2</v>
       </c>
       <c r="I70">
         <v>10</v>
+      </c>
+      <c r="J70" t="s">
+        <v>74</v>
+      </c>
+      <c r="L70" t="str">
+        <f t="shared" si="6"/>
+        <v>frameTotalScoresPlayer2[10]</v>
+      </c>
+      <c r="N70" s="2" t="str">
+        <f t="shared" si="9"/>
+        <v>frame10TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[10]);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="str">
+        <f>A2&amp;B2&amp;";"</f>
+        <v>TextView frame1Score1Player1;</v>
+      </c>
+      <c r="G2" t="str">
+        <f>B2&amp;" = findViewById(R.id."&amp;B2&amp;");"</f>
+        <v>frame1Score1Player1 = findViewById(R.id.frame1Score1Player1);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C63" si="0">A3&amp;B3&amp;";"</f>
+        <v>TextView frame1Score2Player1;</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G63" si="1">B3&amp;" = findViewById(R.id."&amp;B3&amp;");"</f>
+        <v>frame1Score2Player1 = findViewById(R.id.frame1Score2Player1);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame2Score1Player1;</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>frame2Score1Player1 = findViewById(R.id.frame2Score1Player1);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame2Score2Player1;</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>frame2Score2Player1 = findViewById(R.id.frame2Score2Player1);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame3Score1Player1;</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>frame3Score1Player1 = findViewById(R.id.frame3Score1Player1);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame3Score2Player1;</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>frame3Score2Player1 = findViewById(R.id.frame3Score2Player1);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame4Score1Player1;</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>frame4Score1Player1 = findViewById(R.id.frame4Score1Player1);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame4Score2Player1;</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>frame4Score2Player1 = findViewById(R.id.frame4Score2Player1);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame5Score1Player1;</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>frame5Score1Player1 = findViewById(R.id.frame5Score1Player1);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame5Score2Player1;</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>frame5Score2Player1 = findViewById(R.id.frame5Score2Player1);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame6Score1Player1;</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>frame6Score1Player1 = findViewById(R.id.frame6Score1Player1);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame6Score2Player1;</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>frame6Score2Player1 = findViewById(R.id.frame6Score2Player1);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame7Score1Player1;</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>frame7Score1Player1 = findViewById(R.id.frame7Score1Player1);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame7Score2Player1;</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>frame7Score2Player1 = findViewById(R.id.frame7Score2Player1);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame8Score1Player1;</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>frame8Score1Player1 = findViewById(R.id.frame8Score1Player1);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame8Score2Player1;</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>frame8Score2Player1 = findViewById(R.id.frame8Score2Player1);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame9Score1Player1;</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>frame9Score1Player1 = findViewById(R.id.frame9Score1Player1);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame9Score2Player1;</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>frame9Score2Player1 = findViewById(R.id.frame9Score2Player1);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame10Score1Player1;</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>frame10Score1Player1 = findViewById(R.id.frame10Score1Player1);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame10Score2Player1;</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>frame10Score2Player1 = findViewById(R.id.frame10Score2Player1);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame10Score3Player1;</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>frame10Score3Player1 = findViewById(R.id.frame10Score3Player1);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame1Score1Player2;</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>frame1Score1Player2 = findViewById(R.id.frame1Score1Player2);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame1Score2Player2;</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>frame1Score2Player2 = findViewById(R.id.frame1Score2Player2);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame2Score1Player2;</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>frame2Score1Player2 = findViewById(R.id.frame2Score1Player2);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame2Score2Player2;</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v>frame2Score2Player2 = findViewById(R.id.frame2Score2Player2);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame3Score1Player2;</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>frame3Score1Player2 = findViewById(R.id.frame3Score1Player2);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame3Score2Player2;</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v>frame3Score2Player2 = findViewById(R.id.frame3Score2Player2);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame4Score1Player2;</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v>frame4Score1Player2 = findViewById(R.id.frame4Score1Player2);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame4Score2Player2;</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v>frame4Score2Player2 = findViewById(R.id.frame4Score2Player2);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame5Score1Player2;</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v>frame5Score1Player2 = findViewById(R.id.frame5Score1Player2);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame5Score2Player2;</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v>frame5Score2Player2 = findViewById(R.id.frame5Score2Player2);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame6Score1Player2;</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v>frame6Score1Player2 = findViewById(R.id.frame6Score1Player2);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame6Score2Player2;</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v>frame6Score2Player2 = findViewById(R.id.frame6Score2Player2);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame7Score1Player2;</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="1"/>
+        <v>frame7Score1Player2 = findViewById(R.id.frame7Score1Player2);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame7Score2Player2;</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v>frame7Score2Player2 = findViewById(R.id.frame7Score2Player2);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame8Score1Player2;</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v>frame8Score1Player2 = findViewById(R.id.frame8Score1Player2);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame8Score2Player2;</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="1"/>
+        <v>frame8Score2Player2 = findViewById(R.id.frame8Score2Player2);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame9Score1Player2;</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="1"/>
+        <v>frame9Score1Player2 = findViewById(R.id.frame9Score1Player2);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame9Score2Player2;</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v>frame9Score2Player2 = findViewById(R.id.frame9Score2Player2);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame10Score1Player2;</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="1"/>
+        <v>frame10Score1Player2 = findViewById(R.id.frame10Score1Player2);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame10Score2Player2;</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="1"/>
+        <v>frame10Score2Player2 = findViewById(R.id.frame10Score2Player2);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame10Score3Player2;</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="1"/>
+        <v>frame10Score3Player2 = findViewById(R.id.frame10Score3Player2);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame1TotalScorePlayer1;</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="1"/>
+        <v>frame1TotalScorePlayer1 = findViewById(R.id.frame1TotalScorePlayer1);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame2TotalScorePlayer1;</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="1"/>
+        <v>frame2TotalScorePlayer1 = findViewById(R.id.frame2TotalScorePlayer1);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame3TotalScorePlayer1;</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="1"/>
+        <v>frame3TotalScorePlayer1 = findViewById(R.id.frame3TotalScorePlayer1);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame4TotalScorePlayer1;</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="1"/>
+        <v>frame4TotalScorePlayer1 = findViewById(R.id.frame4TotalScorePlayer1);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame5TotalScorePlayer1;</v>
+      </c>
+      <c r="G48" t="str">
+        <f t="shared" si="1"/>
+        <v>frame5TotalScorePlayer1 = findViewById(R.id.frame5TotalScorePlayer1);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame6TotalScorePlayer1;</v>
+      </c>
+      <c r="G49" t="str">
+        <f t="shared" si="1"/>
+        <v>frame6TotalScorePlayer1 = findViewById(R.id.frame6TotalScorePlayer1);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame7TotalScorePlayer1;</v>
+      </c>
+      <c r="G50" t="str">
+        <f t="shared" si="1"/>
+        <v>frame7TotalScorePlayer1 = findViewById(R.id.frame7TotalScorePlayer1);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame8TotalScorePlayer1;</v>
+      </c>
+      <c r="G51" t="str">
+        <f t="shared" si="1"/>
+        <v>frame8TotalScorePlayer1 = findViewById(R.id.frame8TotalScorePlayer1);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame9TotalScorePlayer1;</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" si="1"/>
+        <v>frame9TotalScorePlayer1 = findViewById(R.id.frame9TotalScorePlayer1);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame10TotalScorePlayer1;</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" si="1"/>
+        <v>frame10TotalScorePlayer1 = findViewById(R.id.frame10TotalScorePlayer1);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame1TotalScorePlayer2;</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="1"/>
+        <v>frame1TotalScorePlayer2 = findViewById(R.id.frame1TotalScorePlayer2);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame2TotalScorePlayer2;</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="1"/>
+        <v>frame2TotalScorePlayer2 = findViewById(R.id.frame2TotalScorePlayer2);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame3TotalScorePlayer2;</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="1"/>
+        <v>frame3TotalScorePlayer2 = findViewById(R.id.frame3TotalScorePlayer2);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame4TotalScorePlayer2;</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="1"/>
+        <v>frame4TotalScorePlayer2 = findViewById(R.id.frame4TotalScorePlayer2);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame5TotalScorePlayer2;</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="1"/>
+        <v>frame5TotalScorePlayer2 = findViewById(R.id.frame5TotalScorePlayer2);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame6TotalScorePlayer2;</v>
+      </c>
+      <c r="G59" t="str">
+        <f t="shared" si="1"/>
+        <v>frame6TotalScorePlayer2 = findViewById(R.id.frame6TotalScorePlayer2);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame7TotalScorePlayer2;</v>
+      </c>
+      <c r="G60" t="str">
+        <f t="shared" si="1"/>
+        <v>frame7TotalScorePlayer2 = findViewById(R.id.frame7TotalScorePlayer2);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame8TotalScorePlayer2;</v>
+      </c>
+      <c r="G61" t="str">
+        <f t="shared" si="1"/>
+        <v>frame8TotalScorePlayer2 = findViewById(R.id.frame8TotalScorePlayer2);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B62" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame9TotalScorePlayer2;</v>
+      </c>
+      <c r="G62" t="str">
+        <f t="shared" si="1"/>
+        <v>frame9TotalScorePlayer2 = findViewById(R.id.frame9TotalScorePlayer2);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>TextView frame10TotalScorePlayer2;</v>
+      </c>
+      <c r="G63" t="str">
+        <f t="shared" si="1"/>
+        <v>frame10TotalScorePlayer2 = findViewById(R.id.frame10TotalScorePlayer2);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change strike score display
</commit_message>
<xml_diff>
--- a/variable list.xlsx
+++ b/variable list.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="195">
   <si>
     <t>Score</t>
   </si>
@@ -8412,7 +8412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E37" workbookViewId="0">
       <selection activeCell="M59" sqref="M59:M68"/>
     </sheetView>
   </sheetViews>
@@ -8434,8 +8434,8 @@
         <v>137</v>
       </c>
       <c r="M1" s="3" t="str">
-        <f>"if ("&amp;K1&amp;" == 20) { "&amp;J1&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); } else if ("&amp;K1&amp;" == 30)  { "&amp;J1&amp;".setText("&amp;CHAR(34)&amp;"/"&amp;CHAR(34)&amp;"); } else if ("&amp;K1&amp;" == 40)  { "&amp;J1&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"); } else if ("&amp;K1&amp;" == 0)  { "&amp;J1&amp;".setText("&amp;CHAR(34)&amp;"-"&amp;CHAR(34)&amp;"); }  else {"&amp;J1&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;K1&amp;");}"</f>
-        <v>if (frameScoresPlayer1[1] == 20) { frame1Score1Player1.setText("X"); } else if (frameScoresPlayer1[1] == 30)  { frame1Score1Player1.setText("/"); } else if (frameScoresPlayer1[1] == 40)  { frame1Score1Player1.setText(""); } else if (frameScoresPlayer1[1] == 0)  { frame1Score1Player1.setText("-"); }  else {frame1Score1Player1.setText(""+frameScoresPlayer1[1]);}</v>
+        <f>"if ("&amp;K1&amp;" == 10) { "&amp;J1&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); } else if ("&amp;K1&amp;" == 30)  { "&amp;J1&amp;".setText("&amp;CHAR(34)&amp;"/"&amp;CHAR(34)&amp;"); } else if ("&amp;K1&amp;" == 40)  { "&amp;J1&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"); } else if ("&amp;K1&amp;" == 0)  { "&amp;J1&amp;".setText("&amp;CHAR(34)&amp;"-"&amp;CHAR(34)&amp;"); }  else {"&amp;J1&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;K1&amp;");}"</f>
+        <v>if (frameScoresPlayer1[1] == 10) { frame1Score1Player1.setText("X"); } else if (frameScoresPlayer1[1] == 30)  { frame1Score1Player1.setText("/"); } else if (frameScoresPlayer1[1] == 40)  { frame1Score1Player1.setText(""); } else if (frameScoresPlayer1[1] == 0)  { frame1Score1Player1.setText("-"); }  else {frame1Score1Player1.setText(""+frameScoresPlayer1[1]);}</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -8449,8 +8449,8 @@
         <v>138</v>
       </c>
       <c r="M2" s="3" t="str">
-        <f t="shared" ref="M2:M65" si="0">"if ("&amp;K2&amp;" == 20) { "&amp;J2&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); } else if ("&amp;K2&amp;" == 30)  { "&amp;J2&amp;".setText("&amp;CHAR(34)&amp;"/"&amp;CHAR(34)&amp;"); } else if ("&amp;K2&amp;" == 40)  { "&amp;J2&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"); } else if ("&amp;K2&amp;" == 0)  { "&amp;J2&amp;".setText("&amp;CHAR(34)&amp;"-"&amp;CHAR(34)&amp;"); }  else {"&amp;J2&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;K2&amp;");}"</f>
-        <v>if (frameScoresPlayer1[2] == 20) { frame1Score2Player1.setText("X"); } else if (frameScoresPlayer1[2] == 30)  { frame1Score2Player1.setText("/"); } else if (frameScoresPlayer1[2] == 40)  { frame1Score2Player1.setText(""); } else if (frameScoresPlayer1[2] == 0)  { frame1Score2Player1.setText("-"); }  else {frame1Score2Player1.setText(""+frameScoresPlayer1[2]);}</v>
+        <f t="shared" ref="M2:M65" si="0">"if ("&amp;K2&amp;" == 10) { "&amp;J2&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); } else if ("&amp;K2&amp;" == 30)  { "&amp;J2&amp;".setText("&amp;CHAR(34)&amp;"/"&amp;CHAR(34)&amp;"); } else if ("&amp;K2&amp;" == 40)  { "&amp;J2&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"); } else if ("&amp;K2&amp;" == 0)  { "&amp;J2&amp;".setText("&amp;CHAR(34)&amp;"-"&amp;CHAR(34)&amp;"); }  else {"&amp;J2&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;K2&amp;");}"</f>
+        <v>if (frameScoresPlayer1[2] == 10) { frame1Score2Player1.setText("X"); } else if (frameScoresPlayer1[2] == 30)  { frame1Score2Player1.setText("/"); } else if (frameScoresPlayer1[2] == 40)  { frame1Score2Player1.setText(""); } else if (frameScoresPlayer1[2] == 0)  { frame1Score2Player1.setText("-"); }  else {frame1Score2Player1.setText(""+frameScoresPlayer1[2]);}</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -8465,7 +8465,7 @@
       </c>
       <c r="M3" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[3] == 20) { frame2Score1Player1.setText("X"); } else if (frameScoresPlayer1[3] == 30)  { frame2Score1Player1.setText("/"); } else if (frameScoresPlayer1[3] == 40)  { frame2Score1Player1.setText(""); } else if (frameScoresPlayer1[3] == 0)  { frame2Score1Player1.setText("-"); }  else {frame2Score1Player1.setText(""+frameScoresPlayer1[3]);}</v>
+        <v>if (frameScoresPlayer1[3] == 10) { frame2Score1Player1.setText("X"); } else if (frameScoresPlayer1[3] == 30)  { frame2Score1Player1.setText("/"); } else if (frameScoresPlayer1[3] == 40)  { frame2Score1Player1.setText(""); } else if (frameScoresPlayer1[3] == 0)  { frame2Score1Player1.setText("-"); }  else {frame2Score1Player1.setText(""+frameScoresPlayer1[3]);}</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -8480,7 +8480,7 @@
       </c>
       <c r="M4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[4] == 20) { frame2Score2Player1.setText("X"); } else if (frameScoresPlayer1[4] == 30)  { frame2Score2Player1.setText("/"); } else if (frameScoresPlayer1[4] == 40)  { frame2Score2Player1.setText(""); } else if (frameScoresPlayer1[4] == 0)  { frame2Score2Player1.setText("-"); }  else {frame2Score2Player1.setText(""+frameScoresPlayer1[4]);}</v>
+        <v>if (frameScoresPlayer1[4] == 10) { frame2Score2Player1.setText("X"); } else if (frameScoresPlayer1[4] == 30)  { frame2Score2Player1.setText("/"); } else if (frameScoresPlayer1[4] == 40)  { frame2Score2Player1.setText(""); } else if (frameScoresPlayer1[4] == 0)  { frame2Score2Player1.setText("-"); }  else {frame2Score2Player1.setText(""+frameScoresPlayer1[4]);}</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -8495,7 +8495,7 @@
       </c>
       <c r="M5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[5] == 20) { frame3Score1Player1.setText("X"); } else if (frameScoresPlayer1[5] == 30)  { frame3Score1Player1.setText("/"); } else if (frameScoresPlayer1[5] == 40)  { frame3Score1Player1.setText(""); } else if (frameScoresPlayer1[5] == 0)  { frame3Score1Player1.setText("-"); }  else {frame3Score1Player1.setText(""+frameScoresPlayer1[5]);}</v>
+        <v>if (frameScoresPlayer1[5] == 10) { frame3Score1Player1.setText("X"); } else if (frameScoresPlayer1[5] == 30)  { frame3Score1Player1.setText("/"); } else if (frameScoresPlayer1[5] == 40)  { frame3Score1Player1.setText(""); } else if (frameScoresPlayer1[5] == 0)  { frame3Score1Player1.setText("-"); }  else {frame3Score1Player1.setText(""+frameScoresPlayer1[5]);}</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -8510,7 +8510,7 @@
       </c>
       <c r="M6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[6] == 20) { frame3Score2Player1.setText("X"); } else if (frameScoresPlayer1[6] == 30)  { frame3Score2Player1.setText("/"); } else if (frameScoresPlayer1[6] == 40)  { frame3Score2Player1.setText(""); } else if (frameScoresPlayer1[6] == 0)  { frame3Score2Player1.setText("-"); }  else {frame3Score2Player1.setText(""+frameScoresPlayer1[6]);}</v>
+        <v>if (frameScoresPlayer1[6] == 10) { frame3Score2Player1.setText("X"); } else if (frameScoresPlayer1[6] == 30)  { frame3Score2Player1.setText("/"); } else if (frameScoresPlayer1[6] == 40)  { frame3Score2Player1.setText(""); } else if (frameScoresPlayer1[6] == 0)  { frame3Score2Player1.setText("-"); }  else {frame3Score2Player1.setText(""+frameScoresPlayer1[6]);}</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -8525,7 +8525,7 @@
       </c>
       <c r="M7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[7] == 20) { frame4Score1Player1.setText("X"); } else if (frameScoresPlayer1[7] == 30)  { frame4Score1Player1.setText("/"); } else if (frameScoresPlayer1[7] == 40)  { frame4Score1Player1.setText(""); } else if (frameScoresPlayer1[7] == 0)  { frame4Score1Player1.setText("-"); }  else {frame4Score1Player1.setText(""+frameScoresPlayer1[7]);}</v>
+        <v>if (frameScoresPlayer1[7] == 10) { frame4Score1Player1.setText("X"); } else if (frameScoresPlayer1[7] == 30)  { frame4Score1Player1.setText("/"); } else if (frameScoresPlayer1[7] == 40)  { frame4Score1Player1.setText(""); } else if (frameScoresPlayer1[7] == 0)  { frame4Score1Player1.setText("-"); }  else {frame4Score1Player1.setText(""+frameScoresPlayer1[7]);}</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -8540,7 +8540,7 @@
       </c>
       <c r="M8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[8] == 20) { frame4Score2Player1.setText("X"); } else if (frameScoresPlayer1[8] == 30)  { frame4Score2Player1.setText("/"); } else if (frameScoresPlayer1[8] == 40)  { frame4Score2Player1.setText(""); } else if (frameScoresPlayer1[8] == 0)  { frame4Score2Player1.setText("-"); }  else {frame4Score2Player1.setText(""+frameScoresPlayer1[8]);}</v>
+        <v>if (frameScoresPlayer1[8] == 10) { frame4Score2Player1.setText("X"); } else if (frameScoresPlayer1[8] == 30)  { frame4Score2Player1.setText("/"); } else if (frameScoresPlayer1[8] == 40)  { frame4Score2Player1.setText(""); } else if (frameScoresPlayer1[8] == 0)  { frame4Score2Player1.setText("-"); }  else {frame4Score2Player1.setText(""+frameScoresPlayer1[8]);}</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -8555,7 +8555,7 @@
       </c>
       <c r="M9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[9] == 20) { frame5Score1Player1.setText("X"); } else if (frameScoresPlayer1[9] == 30)  { frame5Score1Player1.setText("/"); } else if (frameScoresPlayer1[9] == 40)  { frame5Score1Player1.setText(""); } else if (frameScoresPlayer1[9] == 0)  { frame5Score1Player1.setText("-"); }  else {frame5Score1Player1.setText(""+frameScoresPlayer1[9]);}</v>
+        <v>if (frameScoresPlayer1[9] == 10) { frame5Score1Player1.setText("X"); } else if (frameScoresPlayer1[9] == 30)  { frame5Score1Player1.setText("/"); } else if (frameScoresPlayer1[9] == 40)  { frame5Score1Player1.setText(""); } else if (frameScoresPlayer1[9] == 0)  { frame5Score1Player1.setText("-"); }  else {frame5Score1Player1.setText(""+frameScoresPlayer1[9]);}</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -8570,7 +8570,7 @@
       </c>
       <c r="M10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[10] == 20) { frame5Score2Player1.setText("X"); } else if (frameScoresPlayer1[10] == 30)  { frame5Score2Player1.setText("/"); } else if (frameScoresPlayer1[10] == 40)  { frame5Score2Player1.setText(""); } else if (frameScoresPlayer1[10] == 0)  { frame5Score2Player1.setText("-"); }  else {frame5Score2Player1.setText(""+frameScoresPlayer1[10]);}</v>
+        <v>if (frameScoresPlayer1[10] == 10) { frame5Score2Player1.setText("X"); } else if (frameScoresPlayer1[10] == 30)  { frame5Score2Player1.setText("/"); } else if (frameScoresPlayer1[10] == 40)  { frame5Score2Player1.setText(""); } else if (frameScoresPlayer1[10] == 0)  { frame5Score2Player1.setText("-"); }  else {frame5Score2Player1.setText(""+frameScoresPlayer1[10]);}</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -8585,7 +8585,7 @@
       </c>
       <c r="M11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[11] == 20) { frame6Score1Player1.setText("X"); } else if (frameScoresPlayer1[11] == 30)  { frame6Score1Player1.setText("/"); } else if (frameScoresPlayer1[11] == 40)  { frame6Score1Player1.setText(""); } else if (frameScoresPlayer1[11] == 0)  { frame6Score1Player1.setText("-"); }  else {frame6Score1Player1.setText(""+frameScoresPlayer1[11]);}</v>
+        <v>if (frameScoresPlayer1[11] == 10) { frame6Score1Player1.setText("X"); } else if (frameScoresPlayer1[11] == 30)  { frame6Score1Player1.setText("/"); } else if (frameScoresPlayer1[11] == 40)  { frame6Score1Player1.setText(""); } else if (frameScoresPlayer1[11] == 0)  { frame6Score1Player1.setText("-"); }  else {frame6Score1Player1.setText(""+frameScoresPlayer1[11]);}</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -8600,7 +8600,7 @@
       </c>
       <c r="M12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[12] == 20) { frame6Score2Player1.setText("X"); } else if (frameScoresPlayer1[12] == 30)  { frame6Score2Player1.setText("/"); } else if (frameScoresPlayer1[12] == 40)  { frame6Score2Player1.setText(""); } else if (frameScoresPlayer1[12] == 0)  { frame6Score2Player1.setText("-"); }  else {frame6Score2Player1.setText(""+frameScoresPlayer1[12]);}</v>
+        <v>if (frameScoresPlayer1[12] == 10) { frame6Score2Player1.setText("X"); } else if (frameScoresPlayer1[12] == 30)  { frame6Score2Player1.setText("/"); } else if (frameScoresPlayer1[12] == 40)  { frame6Score2Player1.setText(""); } else if (frameScoresPlayer1[12] == 0)  { frame6Score2Player1.setText("-"); }  else {frame6Score2Player1.setText(""+frameScoresPlayer1[12]);}</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -8615,7 +8615,7 @@
       </c>
       <c r="M13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[13] == 20) { frame7Score1Player1.setText("X"); } else if (frameScoresPlayer1[13] == 30)  { frame7Score1Player1.setText("/"); } else if (frameScoresPlayer1[13] == 40)  { frame7Score1Player1.setText(""); } else if (frameScoresPlayer1[13] == 0)  { frame7Score1Player1.setText("-"); }  else {frame7Score1Player1.setText(""+frameScoresPlayer1[13]);}</v>
+        <v>if (frameScoresPlayer1[13] == 10) { frame7Score1Player1.setText("X"); } else if (frameScoresPlayer1[13] == 30)  { frame7Score1Player1.setText("/"); } else if (frameScoresPlayer1[13] == 40)  { frame7Score1Player1.setText(""); } else if (frameScoresPlayer1[13] == 0)  { frame7Score1Player1.setText("-"); }  else {frame7Score1Player1.setText(""+frameScoresPlayer1[13]);}</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -8630,7 +8630,7 @@
       </c>
       <c r="M14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[14] == 20) { frame7Score2Player1.setText("X"); } else if (frameScoresPlayer1[14] == 30)  { frame7Score2Player1.setText("/"); } else if (frameScoresPlayer1[14] == 40)  { frame7Score2Player1.setText(""); } else if (frameScoresPlayer1[14] == 0)  { frame7Score2Player1.setText("-"); }  else {frame7Score2Player1.setText(""+frameScoresPlayer1[14]);}</v>
+        <v>if (frameScoresPlayer1[14] == 10) { frame7Score2Player1.setText("X"); } else if (frameScoresPlayer1[14] == 30)  { frame7Score2Player1.setText("/"); } else if (frameScoresPlayer1[14] == 40)  { frame7Score2Player1.setText(""); } else if (frameScoresPlayer1[14] == 0)  { frame7Score2Player1.setText("-"); }  else {frame7Score2Player1.setText(""+frameScoresPlayer1[14]);}</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -8645,7 +8645,7 @@
       </c>
       <c r="M15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[15] == 20) { frame8Score1Player1.setText("X"); } else if (frameScoresPlayer1[15] == 30)  { frame8Score1Player1.setText("/"); } else if (frameScoresPlayer1[15] == 40)  { frame8Score1Player1.setText(""); } else if (frameScoresPlayer1[15] == 0)  { frame8Score1Player1.setText("-"); }  else {frame8Score1Player1.setText(""+frameScoresPlayer1[15]);}</v>
+        <v>if (frameScoresPlayer1[15] == 10) { frame8Score1Player1.setText("X"); } else if (frameScoresPlayer1[15] == 30)  { frame8Score1Player1.setText("/"); } else if (frameScoresPlayer1[15] == 40)  { frame8Score1Player1.setText(""); } else if (frameScoresPlayer1[15] == 0)  { frame8Score1Player1.setText("-"); }  else {frame8Score1Player1.setText(""+frameScoresPlayer1[15]);}</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -8660,7 +8660,7 @@
       </c>
       <c r="M16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[16] == 20) { frame8Score2Player1.setText("X"); } else if (frameScoresPlayer1[16] == 30)  { frame8Score2Player1.setText("/"); } else if (frameScoresPlayer1[16] == 40)  { frame8Score2Player1.setText(""); } else if (frameScoresPlayer1[16] == 0)  { frame8Score2Player1.setText("-"); }  else {frame8Score2Player1.setText(""+frameScoresPlayer1[16]);}</v>
+        <v>if (frameScoresPlayer1[16] == 10) { frame8Score2Player1.setText("X"); } else if (frameScoresPlayer1[16] == 30)  { frame8Score2Player1.setText("/"); } else if (frameScoresPlayer1[16] == 40)  { frame8Score2Player1.setText(""); } else if (frameScoresPlayer1[16] == 0)  { frame8Score2Player1.setText("-"); }  else {frame8Score2Player1.setText(""+frameScoresPlayer1[16]);}</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -8675,7 +8675,7 @@
       </c>
       <c r="M17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[17] == 20) { frame9Score1Player1.setText("X"); } else if (frameScoresPlayer1[17] == 30)  { frame9Score1Player1.setText("/"); } else if (frameScoresPlayer1[17] == 40)  { frame9Score1Player1.setText(""); } else if (frameScoresPlayer1[17] == 0)  { frame9Score1Player1.setText("-"); }  else {frame9Score1Player1.setText(""+frameScoresPlayer1[17]);}</v>
+        <v>if (frameScoresPlayer1[17] == 10) { frame9Score1Player1.setText("X"); } else if (frameScoresPlayer1[17] == 30)  { frame9Score1Player1.setText("/"); } else if (frameScoresPlayer1[17] == 40)  { frame9Score1Player1.setText(""); } else if (frameScoresPlayer1[17] == 0)  { frame9Score1Player1.setText("-"); }  else {frame9Score1Player1.setText(""+frameScoresPlayer1[17]);}</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -8690,7 +8690,7 @@
       </c>
       <c r="M18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[18] == 20) { frame9Score2Player1.setText("X"); } else if (frameScoresPlayer1[18] == 30)  { frame9Score2Player1.setText("/"); } else if (frameScoresPlayer1[18] == 40)  { frame9Score2Player1.setText(""); } else if (frameScoresPlayer1[18] == 0)  { frame9Score2Player1.setText("-"); }  else {frame9Score2Player1.setText(""+frameScoresPlayer1[18]);}</v>
+        <v>if (frameScoresPlayer1[18] == 10) { frame9Score2Player1.setText("X"); } else if (frameScoresPlayer1[18] == 30)  { frame9Score2Player1.setText("/"); } else if (frameScoresPlayer1[18] == 40)  { frame9Score2Player1.setText(""); } else if (frameScoresPlayer1[18] == 0)  { frame9Score2Player1.setText("-"); }  else {frame9Score2Player1.setText(""+frameScoresPlayer1[18]);}</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -8705,7 +8705,7 @@
       </c>
       <c r="M19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[19] == 20) { frame10Score1Player1.setText("X"); } else if (frameScoresPlayer1[19] == 30)  { frame10Score1Player1.setText("/"); } else if (frameScoresPlayer1[19] == 40)  { frame10Score1Player1.setText(""); } else if (frameScoresPlayer1[19] == 0)  { frame10Score1Player1.setText("-"); }  else {frame10Score1Player1.setText(""+frameScoresPlayer1[19]);}</v>
+        <v>if (frameScoresPlayer1[19] == 10) { frame10Score1Player1.setText("X"); } else if (frameScoresPlayer1[19] == 30)  { frame10Score1Player1.setText("/"); } else if (frameScoresPlayer1[19] == 40)  { frame10Score1Player1.setText(""); } else if (frameScoresPlayer1[19] == 0)  { frame10Score1Player1.setText("-"); }  else {frame10Score1Player1.setText(""+frameScoresPlayer1[19]);}</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -8720,7 +8720,7 @@
       </c>
       <c r="M20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[20] == 20) { frame10Score2Player1.setText("X"); } else if (frameScoresPlayer1[20] == 30)  { frame10Score2Player1.setText("/"); } else if (frameScoresPlayer1[20] == 40)  { frame10Score2Player1.setText(""); } else if (frameScoresPlayer1[20] == 0)  { frame10Score2Player1.setText("-"); }  else {frame10Score2Player1.setText(""+frameScoresPlayer1[20]);}</v>
+        <v>if (frameScoresPlayer1[20] == 10) { frame10Score2Player1.setText("X"); } else if (frameScoresPlayer1[20] == 30)  { frame10Score2Player1.setText("/"); } else if (frameScoresPlayer1[20] == 40)  { frame10Score2Player1.setText(""); } else if (frameScoresPlayer1[20] == 0)  { frame10Score2Player1.setText("-"); }  else {frame10Score2Player1.setText(""+frameScoresPlayer1[20]);}</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -8735,7 +8735,7 @@
       </c>
       <c r="M21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer1[21] == 20) { frame10Score3Player1.setText("X"); } else if (frameScoresPlayer1[21] == 30)  { frame10Score3Player1.setText("/"); } else if (frameScoresPlayer1[21] == 40)  { frame10Score3Player1.setText(""); } else if (frameScoresPlayer1[21] == 0)  { frame10Score3Player1.setText("-"); }  else {frame10Score3Player1.setText(""+frameScoresPlayer1[21]);}</v>
+        <v>if (frameScoresPlayer1[21] == 10) { frame10Score3Player1.setText("X"); } else if (frameScoresPlayer1[21] == 30)  { frame10Score3Player1.setText("/"); } else if (frameScoresPlayer1[21] == 40)  { frame10Score3Player1.setText(""); } else if (frameScoresPlayer1[21] == 0)  { frame10Score3Player1.setText("-"); }  else {frame10Score3Player1.setText(""+frameScoresPlayer1[21]);}</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -8762,7 +8762,7 @@
       </c>
       <c r="M24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[1] == 20) { frame1Score1Player2.setText("X"); } else if (frameScoresPlayer2[1] == 30)  { frame1Score1Player2.setText("/"); } else if (frameScoresPlayer2[1] == 40)  { frame1Score1Player2.setText(""); } else if (frameScoresPlayer2[1] == 0)  { frame1Score1Player2.setText("-"); }  else {frame1Score1Player2.setText(""+frameScoresPlayer2[1]);}</v>
+        <v>if (frameScoresPlayer2[1] == 10) { frame1Score1Player2.setText("X"); } else if (frameScoresPlayer2[1] == 30)  { frame1Score1Player2.setText("/"); } else if (frameScoresPlayer2[1] == 40)  { frame1Score1Player2.setText(""); } else if (frameScoresPlayer2[1] == 0)  { frame1Score1Player2.setText("-"); }  else {frame1Score1Player2.setText(""+frameScoresPlayer2[1]);}</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -8777,7 +8777,7 @@
       </c>
       <c r="M25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[2] == 20) { frame1Score2Player2.setText("X"); } else if (frameScoresPlayer2[2] == 30)  { frame1Score2Player2.setText("/"); } else if (frameScoresPlayer2[2] == 40)  { frame1Score2Player2.setText(""); } else if (frameScoresPlayer2[2] == 0)  { frame1Score2Player2.setText("-"); }  else {frame1Score2Player2.setText(""+frameScoresPlayer2[2]);}</v>
+        <v>if (frameScoresPlayer2[2] == 10) { frame1Score2Player2.setText("X"); } else if (frameScoresPlayer2[2] == 30)  { frame1Score2Player2.setText("/"); } else if (frameScoresPlayer2[2] == 40)  { frame1Score2Player2.setText(""); } else if (frameScoresPlayer2[2] == 0)  { frame1Score2Player2.setText("-"); }  else {frame1Score2Player2.setText(""+frameScoresPlayer2[2]);}</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -8792,7 +8792,7 @@
       </c>
       <c r="M26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[3] == 20) { frame2Score1Player2.setText("X"); } else if (frameScoresPlayer2[3] == 30)  { frame2Score1Player2.setText("/"); } else if (frameScoresPlayer2[3] == 40)  { frame2Score1Player2.setText(""); } else if (frameScoresPlayer2[3] == 0)  { frame2Score1Player2.setText("-"); }  else {frame2Score1Player2.setText(""+frameScoresPlayer2[3]);}</v>
+        <v>if (frameScoresPlayer2[3] == 10) { frame2Score1Player2.setText("X"); } else if (frameScoresPlayer2[3] == 30)  { frame2Score1Player2.setText("/"); } else if (frameScoresPlayer2[3] == 40)  { frame2Score1Player2.setText(""); } else if (frameScoresPlayer2[3] == 0)  { frame2Score1Player2.setText("-"); }  else {frame2Score1Player2.setText(""+frameScoresPlayer2[3]);}</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -8807,7 +8807,7 @@
       </c>
       <c r="M27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[4] == 20) { frame2Score2Player2.setText("X"); } else if (frameScoresPlayer2[4] == 30)  { frame2Score2Player2.setText("/"); } else if (frameScoresPlayer2[4] == 40)  { frame2Score2Player2.setText(""); } else if (frameScoresPlayer2[4] == 0)  { frame2Score2Player2.setText("-"); }  else {frame2Score2Player2.setText(""+frameScoresPlayer2[4]);}</v>
+        <v>if (frameScoresPlayer2[4] == 10) { frame2Score2Player2.setText("X"); } else if (frameScoresPlayer2[4] == 30)  { frame2Score2Player2.setText("/"); } else if (frameScoresPlayer2[4] == 40)  { frame2Score2Player2.setText(""); } else if (frameScoresPlayer2[4] == 0)  { frame2Score2Player2.setText("-"); }  else {frame2Score2Player2.setText(""+frameScoresPlayer2[4]);}</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -8822,7 +8822,7 @@
       </c>
       <c r="M28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[5] == 20) { frame3Score1Player2.setText("X"); } else if (frameScoresPlayer2[5] == 30)  { frame3Score1Player2.setText("/"); } else if (frameScoresPlayer2[5] == 40)  { frame3Score1Player2.setText(""); } else if (frameScoresPlayer2[5] == 0)  { frame3Score1Player2.setText("-"); }  else {frame3Score1Player2.setText(""+frameScoresPlayer2[5]);}</v>
+        <v>if (frameScoresPlayer2[5] == 10) { frame3Score1Player2.setText("X"); } else if (frameScoresPlayer2[5] == 30)  { frame3Score1Player2.setText("/"); } else if (frameScoresPlayer2[5] == 40)  { frame3Score1Player2.setText(""); } else if (frameScoresPlayer2[5] == 0)  { frame3Score1Player2.setText("-"); }  else {frame3Score1Player2.setText(""+frameScoresPlayer2[5]);}</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -8837,7 +8837,7 @@
       </c>
       <c r="M29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[6] == 20) { frame3Score2Player2.setText("X"); } else if (frameScoresPlayer2[6] == 30)  { frame3Score2Player2.setText("/"); } else if (frameScoresPlayer2[6] == 40)  { frame3Score2Player2.setText(""); } else if (frameScoresPlayer2[6] == 0)  { frame3Score2Player2.setText("-"); }  else {frame3Score2Player2.setText(""+frameScoresPlayer2[6]);}</v>
+        <v>if (frameScoresPlayer2[6] == 10) { frame3Score2Player2.setText("X"); } else if (frameScoresPlayer2[6] == 30)  { frame3Score2Player2.setText("/"); } else if (frameScoresPlayer2[6] == 40)  { frame3Score2Player2.setText(""); } else if (frameScoresPlayer2[6] == 0)  { frame3Score2Player2.setText("-"); }  else {frame3Score2Player2.setText(""+frameScoresPlayer2[6]);}</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -8852,7 +8852,7 @@
       </c>
       <c r="M30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[7] == 20) { frame4Score1Player2.setText("X"); } else if (frameScoresPlayer2[7] == 30)  { frame4Score1Player2.setText("/"); } else if (frameScoresPlayer2[7] == 40)  { frame4Score1Player2.setText(""); } else if (frameScoresPlayer2[7] == 0)  { frame4Score1Player2.setText("-"); }  else {frame4Score1Player2.setText(""+frameScoresPlayer2[7]);}</v>
+        <v>if (frameScoresPlayer2[7] == 10) { frame4Score1Player2.setText("X"); } else if (frameScoresPlayer2[7] == 30)  { frame4Score1Player2.setText("/"); } else if (frameScoresPlayer2[7] == 40)  { frame4Score1Player2.setText(""); } else if (frameScoresPlayer2[7] == 0)  { frame4Score1Player2.setText("-"); }  else {frame4Score1Player2.setText(""+frameScoresPlayer2[7]);}</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -8867,7 +8867,7 @@
       </c>
       <c r="M31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[8] == 20) { frame4Score2Player2.setText("X"); } else if (frameScoresPlayer2[8] == 30)  { frame4Score2Player2.setText("/"); } else if (frameScoresPlayer2[8] == 40)  { frame4Score2Player2.setText(""); } else if (frameScoresPlayer2[8] == 0)  { frame4Score2Player2.setText("-"); }  else {frame4Score2Player2.setText(""+frameScoresPlayer2[8]);}</v>
+        <v>if (frameScoresPlayer2[8] == 10) { frame4Score2Player2.setText("X"); } else if (frameScoresPlayer2[8] == 30)  { frame4Score2Player2.setText("/"); } else if (frameScoresPlayer2[8] == 40)  { frame4Score2Player2.setText(""); } else if (frameScoresPlayer2[8] == 0)  { frame4Score2Player2.setText("-"); }  else {frame4Score2Player2.setText(""+frameScoresPlayer2[8]);}</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -8882,7 +8882,7 @@
       </c>
       <c r="M32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[9] == 20) { frame5Score1Player2.setText("X"); } else if (frameScoresPlayer2[9] == 30)  { frame5Score1Player2.setText("/"); } else if (frameScoresPlayer2[9] == 40)  { frame5Score1Player2.setText(""); } else if (frameScoresPlayer2[9] == 0)  { frame5Score1Player2.setText("-"); }  else {frame5Score1Player2.setText(""+frameScoresPlayer2[9]);}</v>
+        <v>if (frameScoresPlayer2[9] == 10) { frame5Score1Player2.setText("X"); } else if (frameScoresPlayer2[9] == 30)  { frame5Score1Player2.setText("/"); } else if (frameScoresPlayer2[9] == 40)  { frame5Score1Player2.setText(""); } else if (frameScoresPlayer2[9] == 0)  { frame5Score1Player2.setText("-"); }  else {frame5Score1Player2.setText(""+frameScoresPlayer2[9]);}</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -8897,7 +8897,7 @@
       </c>
       <c r="M33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[10] == 20) { frame5Score2Player2.setText("X"); } else if (frameScoresPlayer2[10] == 30)  { frame5Score2Player2.setText("/"); } else if (frameScoresPlayer2[10] == 40)  { frame5Score2Player2.setText(""); } else if (frameScoresPlayer2[10] == 0)  { frame5Score2Player2.setText("-"); }  else {frame5Score2Player2.setText(""+frameScoresPlayer2[10]);}</v>
+        <v>if (frameScoresPlayer2[10] == 10) { frame5Score2Player2.setText("X"); } else if (frameScoresPlayer2[10] == 30)  { frame5Score2Player2.setText("/"); } else if (frameScoresPlayer2[10] == 40)  { frame5Score2Player2.setText(""); } else if (frameScoresPlayer2[10] == 0)  { frame5Score2Player2.setText("-"); }  else {frame5Score2Player2.setText(""+frameScoresPlayer2[10]);}</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -8912,7 +8912,7 @@
       </c>
       <c r="M34" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[11] == 20) { frame6Score1Player2.setText("X"); } else if (frameScoresPlayer2[11] == 30)  { frame6Score1Player2.setText("/"); } else if (frameScoresPlayer2[11] == 40)  { frame6Score1Player2.setText(""); } else if (frameScoresPlayer2[11] == 0)  { frame6Score1Player2.setText("-"); }  else {frame6Score1Player2.setText(""+frameScoresPlayer2[11]);}</v>
+        <v>if (frameScoresPlayer2[11] == 10) { frame6Score1Player2.setText("X"); } else if (frameScoresPlayer2[11] == 30)  { frame6Score1Player2.setText("/"); } else if (frameScoresPlayer2[11] == 40)  { frame6Score1Player2.setText(""); } else if (frameScoresPlayer2[11] == 0)  { frame6Score1Player2.setText("-"); }  else {frame6Score1Player2.setText(""+frameScoresPlayer2[11]);}</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -8927,7 +8927,7 @@
       </c>
       <c r="M35" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[12] == 20) { frame6Score2Player2.setText("X"); } else if (frameScoresPlayer2[12] == 30)  { frame6Score2Player2.setText("/"); } else if (frameScoresPlayer2[12] == 40)  { frame6Score2Player2.setText(""); } else if (frameScoresPlayer2[12] == 0)  { frame6Score2Player2.setText("-"); }  else {frame6Score2Player2.setText(""+frameScoresPlayer2[12]);}</v>
+        <v>if (frameScoresPlayer2[12] == 10) { frame6Score2Player2.setText("X"); } else if (frameScoresPlayer2[12] == 30)  { frame6Score2Player2.setText("/"); } else if (frameScoresPlayer2[12] == 40)  { frame6Score2Player2.setText(""); } else if (frameScoresPlayer2[12] == 0)  { frame6Score2Player2.setText("-"); }  else {frame6Score2Player2.setText(""+frameScoresPlayer2[12]);}</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -8942,7 +8942,7 @@
       </c>
       <c r="M36" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[13] == 20) { frame7Score1Player2.setText("X"); } else if (frameScoresPlayer2[13] == 30)  { frame7Score1Player2.setText("/"); } else if (frameScoresPlayer2[13] == 40)  { frame7Score1Player2.setText(""); } else if (frameScoresPlayer2[13] == 0)  { frame7Score1Player2.setText("-"); }  else {frame7Score1Player2.setText(""+frameScoresPlayer2[13]);}</v>
+        <v>if (frameScoresPlayer2[13] == 10) { frame7Score1Player2.setText("X"); } else if (frameScoresPlayer2[13] == 30)  { frame7Score1Player2.setText("/"); } else if (frameScoresPlayer2[13] == 40)  { frame7Score1Player2.setText(""); } else if (frameScoresPlayer2[13] == 0)  { frame7Score1Player2.setText("-"); }  else {frame7Score1Player2.setText(""+frameScoresPlayer2[13]);}</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -8957,7 +8957,7 @@
       </c>
       <c r="M37" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[14] == 20) { frame7Score2Player2.setText("X"); } else if (frameScoresPlayer2[14] == 30)  { frame7Score2Player2.setText("/"); } else if (frameScoresPlayer2[14] == 40)  { frame7Score2Player2.setText(""); } else if (frameScoresPlayer2[14] == 0)  { frame7Score2Player2.setText("-"); }  else {frame7Score2Player2.setText(""+frameScoresPlayer2[14]);}</v>
+        <v>if (frameScoresPlayer2[14] == 10) { frame7Score2Player2.setText("X"); } else if (frameScoresPlayer2[14] == 30)  { frame7Score2Player2.setText("/"); } else if (frameScoresPlayer2[14] == 40)  { frame7Score2Player2.setText(""); } else if (frameScoresPlayer2[14] == 0)  { frame7Score2Player2.setText("-"); }  else {frame7Score2Player2.setText(""+frameScoresPlayer2[14]);}</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -8972,7 +8972,7 @@
       </c>
       <c r="M38" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[15] == 20) { frame8Score1Player2.setText("X"); } else if (frameScoresPlayer2[15] == 30)  { frame8Score1Player2.setText("/"); } else if (frameScoresPlayer2[15] == 40)  { frame8Score1Player2.setText(""); } else if (frameScoresPlayer2[15] == 0)  { frame8Score1Player2.setText("-"); }  else {frame8Score1Player2.setText(""+frameScoresPlayer2[15]);}</v>
+        <v>if (frameScoresPlayer2[15] == 10) { frame8Score1Player2.setText("X"); } else if (frameScoresPlayer2[15] == 30)  { frame8Score1Player2.setText("/"); } else if (frameScoresPlayer2[15] == 40)  { frame8Score1Player2.setText(""); } else if (frameScoresPlayer2[15] == 0)  { frame8Score1Player2.setText("-"); }  else {frame8Score1Player2.setText(""+frameScoresPlayer2[15]);}</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -8987,7 +8987,7 @@
       </c>
       <c r="M39" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[16] == 20) { frame8Score2Player2.setText("X"); } else if (frameScoresPlayer2[16] == 30)  { frame8Score2Player2.setText("/"); } else if (frameScoresPlayer2[16] == 40)  { frame8Score2Player2.setText(""); } else if (frameScoresPlayer2[16] == 0)  { frame8Score2Player2.setText("-"); }  else {frame8Score2Player2.setText(""+frameScoresPlayer2[16]);}</v>
+        <v>if (frameScoresPlayer2[16] == 10) { frame8Score2Player2.setText("X"); } else if (frameScoresPlayer2[16] == 30)  { frame8Score2Player2.setText("/"); } else if (frameScoresPlayer2[16] == 40)  { frame8Score2Player2.setText(""); } else if (frameScoresPlayer2[16] == 0)  { frame8Score2Player2.setText("-"); }  else {frame8Score2Player2.setText(""+frameScoresPlayer2[16]);}</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -9002,7 +9002,7 @@
       </c>
       <c r="M40" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[17] == 20) { frame9Score1Player2.setText("X"); } else if (frameScoresPlayer2[17] == 30)  { frame9Score1Player2.setText("/"); } else if (frameScoresPlayer2[17] == 40)  { frame9Score1Player2.setText(""); } else if (frameScoresPlayer2[17] == 0)  { frame9Score1Player2.setText("-"); }  else {frame9Score1Player2.setText(""+frameScoresPlayer2[17]);}</v>
+        <v>if (frameScoresPlayer2[17] == 10) { frame9Score1Player2.setText("X"); } else if (frameScoresPlayer2[17] == 30)  { frame9Score1Player2.setText("/"); } else if (frameScoresPlayer2[17] == 40)  { frame9Score1Player2.setText(""); } else if (frameScoresPlayer2[17] == 0)  { frame9Score1Player2.setText("-"); }  else {frame9Score1Player2.setText(""+frameScoresPlayer2[17]);}</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -9017,7 +9017,7 @@
       </c>
       <c r="M41" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[18] == 20) { frame9Score2Player2.setText("X"); } else if (frameScoresPlayer2[18] == 30)  { frame9Score2Player2.setText("/"); } else if (frameScoresPlayer2[18] == 40)  { frame9Score2Player2.setText(""); } else if (frameScoresPlayer2[18] == 0)  { frame9Score2Player2.setText("-"); }  else {frame9Score2Player2.setText(""+frameScoresPlayer2[18]);}</v>
+        <v>if (frameScoresPlayer2[18] == 10) { frame9Score2Player2.setText("X"); } else if (frameScoresPlayer2[18] == 30)  { frame9Score2Player2.setText("/"); } else if (frameScoresPlayer2[18] == 40)  { frame9Score2Player2.setText(""); } else if (frameScoresPlayer2[18] == 0)  { frame9Score2Player2.setText("-"); }  else {frame9Score2Player2.setText(""+frameScoresPlayer2[18]);}</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -9032,7 +9032,7 @@
       </c>
       <c r="M42" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[19] == 20) { frame10Score1Player2.setText("X"); } else if (frameScoresPlayer2[19] == 30)  { frame10Score1Player2.setText("/"); } else if (frameScoresPlayer2[19] == 40)  { frame10Score1Player2.setText(""); } else if (frameScoresPlayer2[19] == 0)  { frame10Score1Player2.setText("-"); }  else {frame10Score1Player2.setText(""+frameScoresPlayer2[19]);}</v>
+        <v>if (frameScoresPlayer2[19] == 10) { frame10Score1Player2.setText("X"); } else if (frameScoresPlayer2[19] == 30)  { frame10Score1Player2.setText("/"); } else if (frameScoresPlayer2[19] == 40)  { frame10Score1Player2.setText(""); } else if (frameScoresPlayer2[19] == 0)  { frame10Score1Player2.setText("-"); }  else {frame10Score1Player2.setText(""+frameScoresPlayer2[19]);}</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -9047,7 +9047,7 @@
       </c>
       <c r="M43" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[20] == 20) { frame10Score2Player2.setText("X"); } else if (frameScoresPlayer2[20] == 30)  { frame10Score2Player2.setText("/"); } else if (frameScoresPlayer2[20] == 40)  { frame10Score2Player2.setText(""); } else if (frameScoresPlayer2[20] == 0)  { frame10Score2Player2.setText("-"); }  else {frame10Score2Player2.setText(""+frameScoresPlayer2[20]);}</v>
+        <v>if (frameScoresPlayer2[20] == 10) { frame10Score2Player2.setText("X"); } else if (frameScoresPlayer2[20] == 30)  { frame10Score2Player2.setText("/"); } else if (frameScoresPlayer2[20] == 40)  { frame10Score2Player2.setText(""); } else if (frameScoresPlayer2[20] == 0)  { frame10Score2Player2.setText("-"); }  else {frame10Score2Player2.setText(""+frameScoresPlayer2[20]);}</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -9062,7 +9062,7 @@
       </c>
       <c r="M44" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameScoresPlayer2[21] == 20) { frame10Score3Player2.setText("X"); } else if (frameScoresPlayer2[21] == 30)  { frame10Score3Player2.setText("/"); } else if (frameScoresPlayer2[21] == 40)  { frame10Score3Player2.setText(""); } else if (frameScoresPlayer2[21] == 0)  { frame10Score3Player2.setText("-"); }  else {frame10Score3Player2.setText(""+frameScoresPlayer2[21]);}</v>
+        <v>if (frameScoresPlayer2[21] == 10) { frame10Score3Player2.setText("X"); } else if (frameScoresPlayer2[21] == 30)  { frame10Score3Player2.setText("/"); } else if (frameScoresPlayer2[21] == 40)  { frame10Score3Player2.setText(""); } else if (frameScoresPlayer2[21] == 0)  { frame10Score3Player2.setText("-"); }  else {frame10Score3Player2.setText(""+frameScoresPlayer2[21]);}</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -9089,7 +9089,7 @@
       </c>
       <c r="M47" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer1[1] == 20) { frame1TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[1] == 30)  { frame1TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[1] == 40)  { frame1TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[1] == 0)  { frame1TotalScorePlayer1.setText("-"); }  else {frame1TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[1]);}</v>
+        <v>if (frameTotalScoresPlayer1[1] == 10) { frame1TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[1] == 30)  { frame1TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[1] == 40)  { frame1TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[1] == 0)  { frame1TotalScorePlayer1.setText("-"); }  else {frame1TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[1]);}</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -9104,7 +9104,7 @@
       </c>
       <c r="M48" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer1[2] == 20) { frame2TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[2] == 30)  { frame2TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[2] == 40)  { frame2TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[2] == 0)  { frame2TotalScorePlayer1.setText("-"); }  else {frame2TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[2]);}</v>
+        <v>if (frameTotalScoresPlayer1[2] == 10) { frame2TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[2] == 30)  { frame2TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[2] == 40)  { frame2TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[2] == 0)  { frame2TotalScorePlayer1.setText("-"); }  else {frame2TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[2]);}</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -9119,7 +9119,7 @@
       </c>
       <c r="M49" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer1[3] == 20) { frame3TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[3] == 30)  { frame3TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[3] == 40)  { frame3TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[3] == 0)  { frame3TotalScorePlayer1.setText("-"); }  else {frame3TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[3]);}</v>
+        <v>if (frameTotalScoresPlayer1[3] == 10) { frame3TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[3] == 30)  { frame3TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[3] == 40)  { frame3TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[3] == 0)  { frame3TotalScorePlayer1.setText("-"); }  else {frame3TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[3]);}</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -9134,7 +9134,7 @@
       </c>
       <c r="M50" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer1[4] == 20) { frame4TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[4] == 30)  { frame4TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[4] == 40)  { frame4TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[4] == 0)  { frame4TotalScorePlayer1.setText("-"); }  else {frame4TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[4]);}</v>
+        <v>if (frameTotalScoresPlayer1[4] == 10) { frame4TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[4] == 30)  { frame4TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[4] == 40)  { frame4TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[4] == 0)  { frame4TotalScorePlayer1.setText("-"); }  else {frame4TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[4]);}</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -9149,7 +9149,7 @@
       </c>
       <c r="M51" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer1[5] == 20) { frame5TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[5] == 30)  { frame5TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[5] == 40)  { frame5TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[5] == 0)  { frame5TotalScorePlayer1.setText("-"); }  else {frame5TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[5]);}</v>
+        <v>if (frameTotalScoresPlayer1[5] == 10) { frame5TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[5] == 30)  { frame5TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[5] == 40)  { frame5TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[5] == 0)  { frame5TotalScorePlayer1.setText("-"); }  else {frame5TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[5]);}</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -9164,7 +9164,7 @@
       </c>
       <c r="M52" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer1[6] == 20) { frame6TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[6] == 30)  { frame6TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[6] == 40)  { frame6TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[6] == 0)  { frame6TotalScorePlayer1.setText("-"); }  else {frame6TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[6]);}</v>
+        <v>if (frameTotalScoresPlayer1[6] == 10) { frame6TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[6] == 30)  { frame6TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[6] == 40)  { frame6TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[6] == 0)  { frame6TotalScorePlayer1.setText("-"); }  else {frame6TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[6]);}</v>
       </c>
     </row>
     <row r="53" spans="1:13">
@@ -9179,7 +9179,7 @@
       </c>
       <c r="M53" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer1[7] == 20) { frame7TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[7] == 30)  { frame7TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[7] == 40)  { frame7TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[7] == 0)  { frame7TotalScorePlayer1.setText("-"); }  else {frame7TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[7]);}</v>
+        <v>if (frameTotalScoresPlayer1[7] == 10) { frame7TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[7] == 30)  { frame7TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[7] == 40)  { frame7TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[7] == 0)  { frame7TotalScorePlayer1.setText("-"); }  else {frame7TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[7]);}</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -9194,7 +9194,7 @@
       </c>
       <c r="M54" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer1[8] == 20) { frame8TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[8] == 30)  { frame8TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[8] == 40)  { frame8TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[8] == 0)  { frame8TotalScorePlayer1.setText("-"); }  else {frame8TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[8]);}</v>
+        <v>if (frameTotalScoresPlayer1[8] == 10) { frame8TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[8] == 30)  { frame8TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[8] == 40)  { frame8TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[8] == 0)  { frame8TotalScorePlayer1.setText("-"); }  else {frame8TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[8]);}</v>
       </c>
     </row>
     <row r="55" spans="1:13">
@@ -9209,7 +9209,7 @@
       </c>
       <c r="M55" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer1[9] == 20) { frame9TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[9] == 30)  { frame9TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[9] == 40)  { frame9TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[9] == 0)  { frame9TotalScorePlayer1.setText("-"); }  else {frame9TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[9]);}</v>
+        <v>if (frameTotalScoresPlayer1[9] == 10) { frame9TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[9] == 30)  { frame9TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[9] == 40)  { frame9TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[9] == 0)  { frame9TotalScorePlayer1.setText("-"); }  else {frame9TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[9]);}</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -9224,7 +9224,7 @@
       </c>
       <c r="M56" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer1[10] == 20) { frame10TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[10] == 30)  { frame10TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[10] == 40)  { frame10TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[10] == 0)  { frame10TotalScorePlayer1.setText("-"); }  else {frame10TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[10]);}</v>
+        <v>if (frameTotalScoresPlayer1[10] == 10) { frame10TotalScorePlayer1.setText("X"); } else if (frameTotalScoresPlayer1[10] == 30)  { frame10TotalScorePlayer1.setText("/"); } else if (frameTotalScoresPlayer1[10] == 40)  { frame10TotalScorePlayer1.setText(""); } else if (frameTotalScoresPlayer1[10] == 0)  { frame10TotalScorePlayer1.setText("-"); }  else {frame10TotalScorePlayer1.setText(""+frameTotalScoresPlayer1[10]);}</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -9251,7 +9251,7 @@
       </c>
       <c r="M59" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer2[1] == 20) { frame1TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[1] == 30)  { frame1TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[1] == 40)  { frame1TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[1] == 0)  { frame1TotalScorePlayer2.setText("-"); }  else {frame1TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[1]);}</v>
+        <v>if (frameTotalScoresPlayer2[1] == 10) { frame1TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[1] == 30)  { frame1TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[1] == 40)  { frame1TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[1] == 0)  { frame1TotalScorePlayer2.setText("-"); }  else {frame1TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[1]);}</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -9266,7 +9266,7 @@
       </c>
       <c r="M60" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer2[2] == 20) { frame2TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[2] == 30)  { frame2TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[2] == 40)  { frame2TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[2] == 0)  { frame2TotalScorePlayer2.setText("-"); }  else {frame2TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[2]);}</v>
+        <v>if (frameTotalScoresPlayer2[2] == 10) { frame2TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[2] == 30)  { frame2TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[2] == 40)  { frame2TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[2] == 0)  { frame2TotalScorePlayer2.setText("-"); }  else {frame2TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[2]);}</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -9281,7 +9281,7 @@
       </c>
       <c r="M61" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer2[3] == 20) { frame3TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[3] == 30)  { frame3TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[3] == 40)  { frame3TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[3] == 0)  { frame3TotalScorePlayer2.setText("-"); }  else {frame3TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[3]);}</v>
+        <v>if (frameTotalScoresPlayer2[3] == 10) { frame3TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[3] == 30)  { frame3TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[3] == 40)  { frame3TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[3] == 0)  { frame3TotalScorePlayer2.setText("-"); }  else {frame3TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[3]);}</v>
       </c>
     </row>
     <row r="62" spans="1:13">
@@ -9296,7 +9296,7 @@
       </c>
       <c r="M62" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer2[4] == 20) { frame4TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[4] == 30)  { frame4TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[4] == 40)  { frame4TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[4] == 0)  { frame4TotalScorePlayer2.setText("-"); }  else {frame4TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[4]);}</v>
+        <v>if (frameTotalScoresPlayer2[4] == 10) { frame4TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[4] == 30)  { frame4TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[4] == 40)  { frame4TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[4] == 0)  { frame4TotalScorePlayer2.setText("-"); }  else {frame4TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[4]);}</v>
       </c>
     </row>
     <row r="63" spans="1:13">
@@ -9308,7 +9308,7 @@
       </c>
       <c r="M63" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer2[5] == 20) { frame5TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[5] == 30)  { frame5TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[5] == 40)  { frame5TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[5] == 0)  { frame5TotalScorePlayer2.setText("-"); }  else {frame5TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[5]);}</v>
+        <v>if (frameTotalScoresPlayer2[5] == 10) { frame5TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[5] == 30)  { frame5TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[5] == 40)  { frame5TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[5] == 0)  { frame5TotalScorePlayer2.setText("-"); }  else {frame5TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[5]);}</v>
       </c>
     </row>
     <row r="64" spans="1:13">
@@ -9320,7 +9320,7 @@
       </c>
       <c r="M64" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer2[6] == 20) { frame6TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[6] == 30)  { frame6TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[6] == 40)  { frame6TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[6] == 0)  { frame6TotalScorePlayer2.setText("-"); }  else {frame6TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[6]);}</v>
+        <v>if (frameTotalScoresPlayer2[6] == 10) { frame6TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[6] == 30)  { frame6TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[6] == 40)  { frame6TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[6] == 0)  { frame6TotalScorePlayer2.setText("-"); }  else {frame6TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[6]);}</v>
       </c>
     </row>
     <row r="65" spans="10:13">
@@ -9332,7 +9332,7 @@
       </c>
       <c r="M65" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>if (frameTotalScoresPlayer2[7] == 20) { frame7TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[7] == 30)  { frame7TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[7] == 40)  { frame7TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[7] == 0)  { frame7TotalScorePlayer2.setText("-"); }  else {frame7TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[7]);}</v>
+        <v>if (frameTotalScoresPlayer2[7] == 10) { frame7TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[7] == 30)  { frame7TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[7] == 40)  { frame7TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[7] == 0)  { frame7TotalScorePlayer2.setText("-"); }  else {frame7TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[7]);}</v>
       </c>
     </row>
     <row r="66" spans="10:13">
@@ -9343,8 +9343,8 @@
         <v>193</v>
       </c>
       <c r="M66" s="3" t="str">
-        <f t="shared" ref="M66:M68" si="1">"if ("&amp;K66&amp;" == 20) { "&amp;J66&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); } else if ("&amp;K66&amp;" == 30)  { "&amp;J66&amp;".setText("&amp;CHAR(34)&amp;"/"&amp;CHAR(34)&amp;"); } else if ("&amp;K66&amp;" == 40)  { "&amp;J66&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"); } else if ("&amp;K66&amp;" == 0)  { "&amp;J66&amp;".setText("&amp;CHAR(34)&amp;"-"&amp;CHAR(34)&amp;"); }  else {"&amp;J66&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;K66&amp;");}"</f>
-        <v>if (frameTotalScoresPlayer2[8] == 20) { frame8TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[8] == 30)  { frame8TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[8] == 40)  { frame8TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[8] == 0)  { frame8TotalScorePlayer2.setText("-"); }  else {frame8TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[8]);}</v>
+        <f t="shared" ref="M66:M68" si="1">"if ("&amp;K66&amp;" == 10) { "&amp;J66&amp;".setText("&amp;CHAR(34)&amp;"X"&amp;CHAR(34)&amp;"); } else if ("&amp;K66&amp;" == 30)  { "&amp;J66&amp;".setText("&amp;CHAR(34)&amp;"/"&amp;CHAR(34)&amp;"); } else if ("&amp;K66&amp;" == 40)  { "&amp;J66&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"); } else if ("&amp;K66&amp;" == 0)  { "&amp;J66&amp;".setText("&amp;CHAR(34)&amp;"-"&amp;CHAR(34)&amp;"); }  else {"&amp;J66&amp;".setText("&amp;CHAR(34)&amp;CHAR(34)&amp;"+"&amp;K66&amp;");}"</f>
+        <v>if (frameTotalScoresPlayer2[8] == 10) { frame8TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[8] == 30)  { frame8TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[8] == 40)  { frame8TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[8] == 0)  { frame8TotalScorePlayer2.setText("-"); }  else {frame8TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[8]);}</v>
       </c>
     </row>
     <row r="67" spans="10:13">
@@ -9356,7 +9356,7 @@
       </c>
       <c r="M67" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>if (frameTotalScoresPlayer2[9] == 20) { frame9TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[9] == 30)  { frame9TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[9] == 40)  { frame9TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[9] == 0)  { frame9TotalScorePlayer2.setText("-"); }  else {frame9TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[9]);}</v>
+        <v>if (frameTotalScoresPlayer2[9] == 10) { frame9TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[9] == 30)  { frame9TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[9] == 40)  { frame9TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[9] == 0)  { frame9TotalScorePlayer2.setText("-"); }  else {frame9TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[9]);}</v>
       </c>
     </row>
     <row r="68" spans="10:13">
@@ -9368,7 +9368,7 @@
       </c>
       <c r="M68" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>if (frameTotalScoresPlayer2[10] == 20) { frame10TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[10] == 30)  { frame10TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[10] == 40)  { frame10TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[10] == 0)  { frame10TotalScorePlayer2.setText("-"); }  else {frame10TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[10]);}</v>
+        <v>if (frameTotalScoresPlayer2[10] == 10) { frame10TotalScorePlayer2.setText("X"); } else if (frameTotalScoresPlayer2[10] == 30)  { frame10TotalScorePlayer2.setText("/"); } else if (frameTotalScoresPlayer2[10] == 40)  { frame10TotalScorePlayer2.setText(""); } else if (frameTotalScoresPlayer2[10] == 0)  { frame10TotalScorePlayer2.setText("-"); }  else {frame10TotalScorePlayer2.setText(""+frameTotalScoresPlayer2[10]);}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>